<commit_message>
2022.12.08 Kmarket 멤버 api 설계
</commit_message>
<xml_diff>
--- a/Kmarket API 설계.xlsx
+++ b/Kmarket API 설계.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\java1\Desktop\Workspace\Kmarket1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>구분</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원 로그인 화면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품 목록 화면</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,10 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://localhost:8080/Kmarket/member/…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://localhost:8080/Kmarket/product/…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,6 +118,93 @@
   </si>
   <si>
     <t>http://localhost:8080/Kmarket/admin/…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/member/login.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조수빈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조수빈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/member/join.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/member/register.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/member/registerSeller.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 로그인 화면
+- 로그인/세션에 정보 저장
+- 자동 로그인/쿠키 생성
+- 아이디 찾기
+- 비밀번호 찾기/비밀번호 변경
+- 회원가입 페이지로 이동
+- 헤더 링크 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 가입 페이지로 연결하는 링크
+- 개인 구매회원 회원가입 페이지로 연결
+- 판매회원 회원가입 페이지로 연결
+- 헤더 링크 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/Kmarket/member/signup.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>약관 동의 화면
+- 약관 내용 로드
+- 필수 동의 요소 모두 동의 체크했는지 확인하기
+- (개인/판매) 회원 가입 페이지로 연결
+- 헤더 링크 연결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인 회원 회원가입 화면
+- 입력한 정보 유효성 및 중복 검사
+- 필수 정보 모두 기입했는지 검사
+- 우편번호 찾기 페이지 구현
+- 회원가입 완료 후 메인 화면으로 리다이렉트
+- 헤더 링크 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 회원 회원가입 화면
+- 입력한 정보 유효성 및 중복 검사
+- 필수 정보 모두 기입했는지 검사
+- 우편번호 찾기 페이지 구현
+- 회원가입 완료 후 메인 화면으로 리다이렉트
+- 헤더 링크 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -184,7 +263,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -196,6 +275,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -516,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,15 +633,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -562,13 +650,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -577,105 +665,161 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="99" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="99" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
+    <hyperlink ref="B11" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="B8" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097CC9FFAC65EFA45BEA04EBBB60CAD5B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b23439a91ba18143205c49e90ab13d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60114a07b5dc583519299b7a26e1c8b6">
     <xsd:element name="properties">
@@ -789,6 +933,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -796,14 +949,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{305CDDD2-5EEF-4FF9-9584-902F68B12982}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E38BF8-DA76-4FEC-BE1F-43A93506C983}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -815,6 +960,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{305CDDD2-5EEF-4FF9-9584-902F68B12982}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>